<commit_message>
added new lists downloads
</commit_message>
<xml_diff>
--- a/downloads/KB-Liste Brown Swiss.xlsx
+++ b/downloads/KB-Liste Brown Swiss.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Anna\HP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1DB3D42-40CD-4FC1-83DB-2F14BF6418FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{924358A6-6ED3-4943-94A5-8E1359109319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{7B2FEED5-12E0-4430-B0C7-4D2EE0423BFD}"/>
   </bookViews>
@@ -449,11 +449,11 @@
     <xf numFmtId="14" fontId="7" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -770,26 +770,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15D16D8F-C432-497D-8544-61DA9ABD0E3E}">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.42578125" customWidth="1"/>
     <col min="2" max="2" width="8" customWidth="1"/>
-    <col min="3" max="3" width="39.5703125" customWidth="1"/>
-    <col min="4" max="4" width="7" customWidth="1"/>
-    <col min="5" max="5" width="7.42578125" customWidth="1"/>
+    <col min="3" max="3" width="39.85546875" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" customWidth="1"/>
+    <col min="5" max="5" width="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
+      <c r="B1" s="21"/>
       <c r="C1" s="16">
-        <v>44519</v>
+        <v>44533</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1034,7 +1034,7 @@
       <c r="B17" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="C17" s="19" t="s">
         <v>78</v>
       </c>
       <c r="D17" s="8">

</xml_diff>